<commit_message>
Updated manual topic evaluation. Updated firebase output. Added some documentation
</commit_message>
<xml_diff>
--- a/topic-files/Manual_Topic_Evaluation.xlsx
+++ b/topic-files/Manual_Topic_Evaluation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktuoh\Documents\School\MCS-DS\CS_410_Text_Info_Systems\Project\CourseProject\topic-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/creon/Desktop/UIUC/CS410/Team Project/CourseProject/topic-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727457C3-E630-4923-90F0-E2AF869D0F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DBD0A5-F79E-4A48-8D5D-6B9B504C16CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{78298D7E-DD7A-4237-BADD-8FAFD49C0CC1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="45980" windowHeight="25360" activeTab="1" xr2:uid="{78298D7E-DD7A-4237-BADD-8FAFD49C0CC1}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -559,39 +559,88 @@
   <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -601,57 +650,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -974,29 +974,29 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -1011,88 +1011,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB3E96CE-B931-4949-8E91-1560B9070820}">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="55.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="53.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="46.5703125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="46.5" customWidth="1"/>
+    <col min="8" max="8" width="21.5" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="21" t="s">
         <v>10</v>
       </c>
       <c r="I1" s="22"/>
       <c r="J1" s="22"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="23" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="14">
         <v>14</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="30" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
@@ -1101,38 +1101,40 @@
       <c r="G3" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="18"/>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="4" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="18"/>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="7" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="29" t="s">
         <v>14</v>
       </c>
       <c r="F5" t="s">
@@ -1141,40 +1143,42 @@
       <c r="G5" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="27" t="s">
+      <c r="I5" s="23"/>
+      <c r="J5" s="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="31"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="H6" s="37"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="33">
+      <c r="C7" s="17"/>
+      <c r="D7" s="13">
         <v>36</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="30" t="s">
         <v>23</v>
       </c>
       <c r="F7" t="s">
@@ -1183,63 +1187,65 @@
       <c r="G7" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="25">
         <v>4</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="18"/>
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="5"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="30"/>
       <c r="F8" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="18"/>
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="5"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="30"/>
       <c r="F9" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="18"/>
       <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="4" t="s">
+      <c r="C10" s="18"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="7" t="s">
+      <c r="G10" s="2"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="29" t="s">
         <v>26</v>
       </c>
       <c r="F11" t="s">
@@ -1248,50 +1254,52 @@
       <c r="G11" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="26">
         <v>2</v>
       </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="5"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="30"/>
       <c r="F12" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="17"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="27" t="s">
+      <c r="H12" s="25"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="G13" s="7"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+    </row>
+    <row r="14" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
         <v>29</v>
       </c>
       <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="33">
+      <c r="C14" s="17"/>
+      <c r="D14" s="13">
         <v>18</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="30" t="s">
         <v>31</v>
       </c>
       <c r="F14" t="s">
@@ -1300,66 +1308,68 @@
       <c r="G14" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H14" s="25">
         <v>4</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="18"/>
       <c r="B15" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="5"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="30"/>
       <c r="F15" t="s">
         <v>33</v>
       </c>
       <c r="G15" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="17"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="18"/>
       <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="5"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="30"/>
       <c r="F16" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="17"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="18"/>
       <c r="B17" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="4" t="s">
+      <c r="C17" s="18"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="7" t="s">
+      <c r="G17" s="2"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="29" t="s">
         <v>51</v>
       </c>
       <c r="F18" t="s">
@@ -1368,72 +1378,76 @@
       <c r="G18" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="16">
+      <c r="H18" s="26">
         <v>3</v>
       </c>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="27" t="s">
+      <c r="I18" s="23"/>
+      <c r="J18" s="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="30" t="s">
+      <c r="G19" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H19" s="34"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="H19" s="27"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+    </row>
+    <row r="20" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="17" t="s">
         <v>38</v>
       </c>
       <c r="B20" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="33">
+      <c r="C20" s="17"/>
+      <c r="D20" s="13">
         <v>30</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="30" t="s">
         <v>43</v>
       </c>
       <c r="F20" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="17">
+      <c r="H20" s="25">
         <v>1</v>
       </c>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="18"/>
       <c r="B21" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="4" t="s">
+      <c r="C21" s="18"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="7" t="s">
+      <c r="G21" s="2"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="29" t="s">
         <v>52</v>
       </c>
       <c r="F22" t="s">
@@ -1442,50 +1456,52 @@
       <c r="G22" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="16">
+      <c r="H22" s="26">
         <v>2</v>
       </c>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="5"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="30"/>
       <c r="F23" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="17"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="26"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="27" t="s">
+      <c r="H23" s="25"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+    </row>
+    <row r="24" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="19"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="30"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
+      <c r="G24" s="7"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+    </row>
+    <row r="25" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
         <v>55</v>
       </c>
       <c r="B25" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="33">
+      <c r="C25" s="17"/>
+      <c r="D25" s="13">
         <v>16</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="30" t="s">
         <v>56</v>
       </c>
       <c r="F25" t="s">
@@ -1494,146 +1510,152 @@
       <c r="G25" t="s">
         <v>59</v>
       </c>
-      <c r="H25" s="17">
+      <c r="H25" s="25">
         <v>2</v>
       </c>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="18"/>
       <c r="B26" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="5"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="30"/>
       <c r="F26" t="s">
         <v>57</v>
       </c>
-      <c r="H26" s="17"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="18"/>
       <c r="B27" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="4" t="s">
+      <c r="C27" s="18"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G27" s="4"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="7" t="s">
+      <c r="G27" s="2"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="29" t="s">
         <v>60</v>
       </c>
       <c r="F28" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="16">
+      <c r="H28" s="26">
         <v>1</v>
       </c>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="5"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="30"/>
       <c r="F29" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="17"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="26"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="27" t="s">
+      <c r="H29" s="25"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+    </row>
+    <row r="30" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G30" s="30"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
+      <c r="G30" s="7"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+    </row>
+    <row r="31" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="17" t="s">
         <v>62</v>
       </c>
       <c r="B31" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="D31" s="33">
+      <c r="D31" s="13">
         <v>136</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="30" t="s">
         <v>64</v>
       </c>
       <c r="F31" t="s">
         <v>66</v>
       </c>
-      <c r="H31" s="17">
+      <c r="H31" s="25">
         <v>1</v>
       </c>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="18"/>
       <c r="B32" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="5"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="30"/>
       <c r="F32" t="s">
         <v>24</v>
       </c>
-      <c r="H32" s="17"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="18"/>
       <c r="B33" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="4" t="s">
+      <c r="C33" s="18"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G33" s="4"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="7" t="s">
+      <c r="G33" s="2"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="29" t="s">
         <v>68</v>
       </c>
       <c r="F34" t="s">
@@ -1642,50 +1664,52 @@
       <c r="G34" t="s">
         <v>72</v>
       </c>
-      <c r="H34" s="16">
+      <c r="H34" s="26">
         <v>2</v>
       </c>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="5"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="30"/>
       <c r="F35" t="s">
         <v>41</v>
       </c>
-      <c r="H35" s="17"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="26"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="27" t="s">
+      <c r="H35" s="25"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+    </row>
+    <row r="36" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="19"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G36" s="30"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="28"/>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="32" t="s">
+      <c r="G36" s="7"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+    </row>
+    <row r="37" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="17" t="s">
         <v>73</v>
       </c>
       <c r="B37" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="32"/>
-      <c r="D37" s="33">
+      <c r="C37" s="17"/>
+      <c r="D37" s="13">
         <v>9</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="30" t="s">
         <v>77</v>
       </c>
       <c r="F37" t="s">
@@ -1694,51 +1718,53 @@
       <c r="G37" t="s">
         <v>81</v>
       </c>
-      <c r="H37" s="17">
+      <c r="H37" s="25">
         <v>3</v>
       </c>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="18"/>
       <c r="B38" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="5"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="30"/>
       <c r="F38" t="s">
         <v>79</v>
       </c>
-      <c r="H38" s="17"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="18"/>
       <c r="B39" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="4" t="s">
+      <c r="C39" s="18"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G39" s="4"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="18"/>
       <c r="B40" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="7" t="s">
+      <c r="C40" s="18"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="29" t="s">
         <v>82</v>
       </c>
       <c r="F40" t="s">
@@ -1747,88 +1773,92 @@
       <c r="G40" t="s">
         <v>85</v>
       </c>
-      <c r="H40" s="16">
+      <c r="H40" s="26">
         <v>4</v>
       </c>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="18"/>
       <c r="B41" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="5"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="30"/>
       <c r="F41" t="s">
         <v>39</v>
       </c>
-      <c r="H41" s="17"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
-    </row>
-    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="26"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="27" t="s">
+      <c r="H41" s="25"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+    </row>
+    <row r="42" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="19"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="G42" s="30"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="28"/>
-    </row>
-    <row r="43" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="32" t="s">
+      <c r="G42" s="7"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+    </row>
+    <row r="43" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="17" t="s">
         <v>86</v>
       </c>
       <c r="B43" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="32"/>
-      <c r="D43" s="33">
+      <c r="C43" s="17"/>
+      <c r="D43" s="13">
         <v>25</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" s="30" t="s">
         <v>87</v>
       </c>
       <c r="F43" t="s">
         <v>74</v>
       </c>
-      <c r="H43" s="17">
+      <c r="H43" s="25">
         <v>1</v>
       </c>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="18"/>
       <c r="B44" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="4" t="s">
+      <c r="C44" s="18"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G44" s="4"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="10"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="18"/>
       <c r="B45" t="s">
         <v>94</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="7" t="s">
+      <c r="C45" s="18"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="29" t="s">
         <v>89</v>
       </c>
       <c r="F45" t="s">
@@ -1837,74 +1867,76 @@
       <c r="G45" t="s">
         <v>92</v>
       </c>
-      <c r="H45" s="16">
+      <c r="H45" s="26">
         <v>4</v>
       </c>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="5"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="30"/>
       <c r="F46" t="s">
         <v>36</v>
       </c>
-      <c r="H46" s="17"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="5"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="30"/>
       <c r="F47" t="s">
         <v>90</v>
       </c>
-      <c r="H47" s="17"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="5"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="30"/>
       <c r="F48" t="s">
         <v>80</v>
       </c>
-      <c r="H48" s="17"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="9"/>
-    </row>
-    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="26"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="27" t="s">
+      <c r="H48" s="25"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+    </row>
+    <row r="49" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="19"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="G49" s="30"/>
-      <c r="H49" s="34"/>
-      <c r="I49" s="28"/>
-      <c r="J49" s="28"/>
-    </row>
-    <row r="50" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="32" t="s">
+      <c r="G49" s="7"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
+    </row>
+    <row r="50" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="17" t="s">
         <v>95</v>
       </c>
       <c r="B50" t="s">
         <v>39</v>
       </c>
-      <c r="C50" s="32"/>
-      <c r="D50" s="33">
+      <c r="C50" s="17"/>
+      <c r="D50" s="13">
         <v>79</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="E50" s="30" t="s">
         <v>96</v>
       </c>
       <c r="F50" t="s">
@@ -1913,87 +1945,91 @@
       <c r="G50" t="s">
         <v>98</v>
       </c>
-      <c r="H50" s="17">
+      <c r="H50" s="25">
         <v>4</v>
       </c>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="18"/>
       <c r="B51" t="s">
         <v>94</v>
       </c>
-      <c r="C51" s="3"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="4" t="s">
+      <c r="C51" s="18"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G51" s="4"/>
-      <c r="H51" s="18"/>
-      <c r="I51" s="10"/>
-      <c r="J51" s="10"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="24"/>
+      <c r="J51" s="24"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="18"/>
       <c r="B52" t="s">
         <v>76</v>
       </c>
-      <c r="C52" s="3"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="7" t="s">
+      <c r="C52" s="18"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="29" t="s">
         <v>99</v>
       </c>
       <c r="F52" t="s">
         <v>18</v>
       </c>
-      <c r="H52" s="16">
+      <c r="H52" s="26">
         <v>1</v>
       </c>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="5"/>
+      <c r="I52" s="23"/>
+      <c r="J52" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="30"/>
       <c r="F53" t="s">
         <v>58</v>
       </c>
-      <c r="H53" s="17"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="9"/>
-    </row>
-    <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="26"/>
-      <c r="B54" s="27"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="27" t="s">
+      <c r="H53" s="25"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+    </row>
+    <row r="54" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="19"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="G54" s="30"/>
-      <c r="H54" s="34"/>
-      <c r="I54" s="28"/>
-      <c r="J54" s="28"/>
-    </row>
-    <row r="55" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="G54" s="7"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+    </row>
+    <row r="55" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="20" t="s">
         <v>101</v>
       </c>
       <c r="B55" t="s">
         <v>74</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="D55" s="12">
+      <c r="D55" s="16">
         <v>55</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E55" s="30" t="s">
         <v>104</v>
       </c>
       <c r="F55" t="s">
@@ -2002,163 +2038,146 @@
       <c r="G55" t="s">
         <v>105</v>
       </c>
-      <c r="H55" s="17">
+      <c r="H55" s="25">
         <v>4</v>
       </c>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="20"/>
       <c r="B56" t="s">
         <v>103</v>
       </c>
-      <c r="C56" s="1"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="5"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="30"/>
       <c r="F56" t="s">
         <v>103</v>
       </c>
-      <c r="H56" s="17"/>
-      <c r="I56" s="9"/>
-      <c r="J56" s="9"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
+      <c r="H56" s="25"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="20"/>
       <c r="B57" t="s">
         <v>76</v>
       </c>
-      <c r="C57" s="1"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="5"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="30"/>
       <c r="F57" t="s">
         <v>76</v>
       </c>
-      <c r="H57" s="17"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
+      <c r="H57" s="25"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="20"/>
       <c r="B58" t="s">
         <v>22</v>
       </c>
-      <c r="C58" s="1"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="4" t="s">
+      <c r="C58" s="20"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G58" s="4"/>
-      <c r="H58" s="18"/>
-      <c r="I58" s="10"/>
-      <c r="J58" s="10"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="8" t="s">
+      <c r="G58" s="2"/>
+      <c r="H58" s="28"/>
+      <c r="I58" s="24"/>
+      <c r="J58" s="24"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="33" t="s">
         <v>107</v>
       </c>
       <c r="F59" t="s">
         <v>74</v>
       </c>
-      <c r="H59" s="17">
+      <c r="H59" s="25">
         <v>5</v>
       </c>
-      <c r="I59" s="12"/>
-      <c r="J59" s="12"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="8"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="20"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="33"/>
       <c r="F60" t="s">
         <v>103</v>
       </c>
-      <c r="H60" s="17"/>
-      <c r="I60" s="12"/>
-      <c r="J60" s="12"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="8"/>
+      <c r="H60" s="25"/>
+      <c r="I60" s="16"/>
+      <c r="J60" s="16"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="20"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="33"/>
       <c r="F61" t="s">
         <v>76</v>
       </c>
-      <c r="H61" s="17"/>
-      <c r="I61" s="12"/>
-      <c r="J61" s="12"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="8"/>
+      <c r="H61" s="25"/>
+      <c r="I61" s="16"/>
+      <c r="J61" s="16"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="20"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="33"/>
       <c r="F62" t="s">
         <v>22</v>
       </c>
-      <c r="H62" s="17"/>
-      <c r="I62" s="12"/>
-      <c r="J62" s="12"/>
+      <c r="H62" s="25"/>
+      <c r="I62" s="16"/>
+      <c r="J62" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="116">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="D37:D42"/>
-    <mergeCell ref="D43:D49"/>
-    <mergeCell ref="D50:D54"/>
-    <mergeCell ref="D55:D62"/>
-    <mergeCell ref="C31:C36"/>
-    <mergeCell ref="C55:C62"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="D7:D13"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="D20:D24"/>
-    <mergeCell ref="D25:D30"/>
-    <mergeCell ref="D31:D36"/>
-    <mergeCell ref="I52:I54"/>
-    <mergeCell ref="J52:J54"/>
-    <mergeCell ref="I55:I58"/>
-    <mergeCell ref="J55:J58"/>
-    <mergeCell ref="I59:I62"/>
-    <mergeCell ref="J59:J62"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="J43:J44"/>
-    <mergeCell ref="I45:I49"/>
-    <mergeCell ref="J45:J49"/>
-    <mergeCell ref="I50:I51"/>
-    <mergeCell ref="J50:J51"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J34:J36"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="I40:I42"/>
-    <mergeCell ref="J40:J42"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="J25:J27"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="J31:J33"/>
-    <mergeCell ref="J14:J17"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="I22:I24"/>
-    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="A55:A62"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="C7:C13"/>
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="C25:C30"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A25:A30"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="E14:E17"/>
     <mergeCell ref="H59:H62"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="J3:J4"/>
@@ -2181,49 +2200,70 @@
     <mergeCell ref="H31:H33"/>
     <mergeCell ref="H34:H36"/>
     <mergeCell ref="H37:H39"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I59:I62"/>
+    <mergeCell ref="J59:J62"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="J43:J44"/>
+    <mergeCell ref="I45:I49"/>
+    <mergeCell ref="J45:J49"/>
+    <mergeCell ref="I50:I51"/>
+    <mergeCell ref="J50:J51"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="I40:I42"/>
+    <mergeCell ref="J40:J42"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="D7:D13"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="D20:D24"/>
+    <mergeCell ref="D25:D30"/>
+    <mergeCell ref="D31:D36"/>
+    <mergeCell ref="I52:I54"/>
+    <mergeCell ref="J52:J54"/>
+    <mergeCell ref="I55:I58"/>
+    <mergeCell ref="J55:J58"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="J31:J33"/>
+    <mergeCell ref="J14:J17"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="I22:I24"/>
+    <mergeCell ref="J22:J24"/>
     <mergeCell ref="E52:E54"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="D37:D42"/>
+    <mergeCell ref="D43:D49"/>
+    <mergeCell ref="D50:D54"/>
+    <mergeCell ref="D55:D62"/>
+    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="C55:C62"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="E55:E58"/>
     <mergeCell ref="E59:E62"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="E37:E39"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="E43:E44"/>
     <mergeCell ref="E45:E49"/>
     <mergeCell ref="E50:E51"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="E31:E33"/>
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="E14:E17"/>
     <mergeCell ref="A31:A36"/>
     <mergeCell ref="A37:A42"/>
     <mergeCell ref="A43:A49"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="A55:A62"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="C7:C13"/>
-    <mergeCell ref="C14:C19"/>
-    <mergeCell ref="C20:C24"/>
-    <mergeCell ref="C25:C30"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A25:A30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E7" r:id="rId1" xr:uid="{DF6C5B22-B422-410A-B22A-3B4DEF6A512C}"/>

</xml_diff>

<commit_message>
updated relevancy for tags vs. document
</commit_message>
<xml_diff>
--- a/topic-files/Manual_Topic_Evaluation.xlsx
+++ b/topic-files/Manual_Topic_Evaluation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/creon/Desktop/UIUC/CS410/Team Project/CourseProject/topic-files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SABreyals\CourseProject\topic-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DBD0A5-F79E-4A48-8D5D-6B9B504C16CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC0CD3B-F5A5-4B5D-B1B8-8740CEB567FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="45980" windowHeight="25360" activeTab="1" xr2:uid="{78298D7E-DD7A-4237-BADD-8FAFD49C0CC1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{78298D7E-DD7A-4237-BADD-8FAFD49C0CC1}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="117">
   <si>
     <t>Topic</t>
   </si>
@@ -383,6 +383,9 @@
   </si>
   <si>
     <t>Projects ultimately selected from: https://github.com/CS410Assignments/CourseProject/network/members</t>
+  </si>
+  <si>
+    <t>4 (topic model)</t>
   </si>
 </sst>
 </file>
@@ -556,7 +559,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -572,85 +575,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -974,29 +983,29 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -1011,64 +1020,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB3E96CE-B931-4949-8E91-1560B9070820}">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L57" sqref="L57"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25:I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="53.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="46.5" customWidth="1"/>
-    <col min="8" max="8" width="21.5" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="46.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="33" t="s">
         <v>69</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="10"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="34"/>
       <c r="B2" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="9"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="33"/>
       <c r="F2" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G2" s="12"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1079,20 +1088,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="21">
         <v>14</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="18" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
@@ -1101,40 +1110,42 @@
       <c r="G3" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14">
+      <c r="I3" s="21">
+        <v>2</v>
+      </c>
+      <c r="J3" s="21">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
+    <row r="4" spans="1:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="32"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="35"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="18"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="29" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="17" t="s">
         <v>14</v>
       </c>
       <c r="F5" t="s">
@@ -1143,42 +1154,44 @@
       <c r="G5" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="23"/>
+      <c r="I5" s="23">
+        <v>2</v>
+      </c>
       <c r="J5" s="23">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+    <row r="6" spans="1:10" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="31"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="37"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-    </row>
-    <row r="7" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="H6" s="28"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="13">
+      <c r="C7" s="9"/>
+      <c r="D7" s="32">
         <v>36</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="18" t="s">
         <v>23</v>
       </c>
       <c r="F7" t="s">
@@ -1187,65 +1200,67 @@
       <c r="G7" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="13">
         <v>4</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14">
+      <c r="I7" s="21">
+        <v>3</v>
+      </c>
+      <c r="J7" s="21">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="30"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="18"/>
       <c r="F8" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="30"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="18"/>
       <c r="F9" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="25"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
       <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="32"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G10" s="2"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="29" t="s">
+      <c r="H10" s="14"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="17" t="s">
         <v>26</v>
       </c>
       <c r="F11" t="s">
@@ -1254,52 +1269,54 @@
       <c r="G11" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="26">
+      <c r="H11" s="15">
         <v>2</v>
       </c>
-      <c r="I11" s="23"/>
+      <c r="I11" s="23">
+        <v>1</v>
+      </c>
       <c r="J11" s="23">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="30"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="18"/>
       <c r="F12" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="25"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-    </row>
-    <row r="13" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="31"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="19"/>
       <c r="F13" s="6" t="s">
         <v>28</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-    </row>
-    <row r="14" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
+      <c r="H13" s="16"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="13">
+      <c r="C14" s="9"/>
+      <c r="D14" s="32">
         <v>18</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="18" t="s">
         <v>31</v>
       </c>
       <c r="F14" t="s">
@@ -1308,68 +1325,70 @@
       <c r="G14" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="13">
         <v>4</v>
       </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14">
+      <c r="I14" s="21">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
+      <c r="J14" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
       <c r="B15" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="30"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="18"/>
       <c r="F15" t="s">
         <v>33</v>
       </c>
       <c r="G15" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
       <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="30"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="18"/>
       <c r="F16" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="25"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
       <c r="B17" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="32"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G17" s="2"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="29" t="s">
+      <c r="H17" s="14"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="17" t="s">
         <v>51</v>
       </c>
       <c r="F18" t="s">
@@ -1378,76 +1397,80 @@
       <c r="G18" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="26">
+      <c r="H18" s="15">
         <v>3</v>
       </c>
-      <c r="I18" s="23"/>
+      <c r="I18" s="23">
+        <v>4</v>
+      </c>
       <c r="J18" s="23">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="31"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="19"/>
       <c r="F19" s="6" t="s">
         <v>37</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H19" s="27"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-    </row>
-    <row r="20" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
+      <c r="H19" s="16"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B20" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="13">
+      <c r="C20" s="9"/>
+      <c r="D20" s="32">
         <v>30</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="18" t="s">
         <v>43</v>
       </c>
       <c r="F20" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="25">
+      <c r="H20" s="13">
         <v>1</v>
       </c>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14">
+      <c r="I20" s="38">
+        <v>1</v>
+      </c>
+      <c r="J20" s="21">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
+    <row r="21" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
       <c r="B21" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="32"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="20"/>
       <c r="F21" s="2" t="s">
         <v>42</v>
       </c>
       <c r="G21" s="2"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="29" t="s">
+      <c r="H21" s="14"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="22"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="17" t="s">
         <v>52</v>
       </c>
       <c r="F22" t="s">
@@ -1456,52 +1479,54 @@
       <c r="G22" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="26">
+      <c r="H22" s="15">
         <v>2</v>
       </c>
-      <c r="I22" s="23"/>
+      <c r="I22" s="23" t="s">
+        <v>116</v>
+      </c>
       <c r="J22" s="23">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="30"/>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="18"/>
       <c r="F23" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="25"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-    </row>
-    <row r="24" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="31"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="19"/>
       <c r="F24" s="6" t="s">
         <v>53</v>
       </c>
       <c r="G24" s="7"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-    </row>
-    <row r="25" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
+      <c r="H24" s="16"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B25" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="13">
+      <c r="C25" s="9"/>
+      <c r="D25" s="32">
         <v>16</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E25" s="18" t="s">
         <v>56</v>
       </c>
       <c r="F25" t="s">
@@ -1510,152 +1535,158 @@
       <c r="G25" t="s">
         <v>59</v>
       </c>
-      <c r="H25" s="25">
+      <c r="H25" s="13">
         <v>2</v>
       </c>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14">
+      <c r="I25" s="21">
+        <v>2</v>
+      </c>
+      <c r="J25" s="21">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
       <c r="B26" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="30"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="18"/>
       <c r="F26" t="s">
         <v>57</v>
       </c>
-      <c r="H26" s="25"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="18"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
       <c r="B27" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="32"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="20"/>
       <c r="F27" s="2" t="s">
         <v>58</v>
       </c>
       <c r="G27" s="2"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="29" t="s">
+      <c r="H27" s="14"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="17" t="s">
         <v>60</v>
       </c>
       <c r="F28" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="26">
+      <c r="H28" s="15">
         <v>1</v>
       </c>
-      <c r="I28" s="23"/>
+      <c r="I28" s="23">
+        <v>1</v>
+      </c>
       <c r="J28" s="23">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="30"/>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="18"/>
       <c r="F29" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="25"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-    </row>
-    <row r="30" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="11"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="31"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="19"/>
       <c r="F30" s="6" t="s">
         <v>61</v>
       </c>
       <c r="G30" s="7"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-    </row>
-    <row r="31" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="17" t="s">
+      <c r="H30" s="16"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>62</v>
       </c>
       <c r="B31" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="32">
         <v>136</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="18" t="s">
         <v>64</v>
       </c>
       <c r="F31" t="s">
         <v>66</v>
       </c>
-      <c r="H31" s="25">
+      <c r="H31" s="13">
         <v>1</v>
       </c>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14">
+      <c r="I31" s="21">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="18"/>
+      <c r="J31" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
       <c r="B32" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="30"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="18"/>
       <c r="F32" t="s">
         <v>24</v>
       </c>
-      <c r="H32" s="25"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="18"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
       <c r="B33" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="32"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="20"/>
       <c r="F33" s="2" t="s">
         <v>67</v>
       </c>
       <c r="G33" s="2"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="29" t="s">
+      <c r="H33" s="14"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="17" t="s">
         <v>68</v>
       </c>
       <c r="F34" t="s">
@@ -1664,52 +1695,54 @@
       <c r="G34" t="s">
         <v>72</v>
       </c>
-      <c r="H34" s="26">
+      <c r="H34" s="15">
         <v>2</v>
       </c>
-      <c r="I34" s="23"/>
+      <c r="I34" s="23">
+        <v>2</v>
+      </c>
       <c r="J34" s="23">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="30"/>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="18"/>
       <c r="F35" t="s">
         <v>41</v>
       </c>
-      <c r="H35" s="25"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-    </row>
-    <row r="36" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="11"/>
       <c r="B36" s="6"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="31"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="19"/>
       <c r="F36" s="6" t="s">
         <v>71</v>
       </c>
       <c r="G36" s="7"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-    </row>
-    <row r="37" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="17" t="s">
+      <c r="H36" s="16"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
         <v>73</v>
       </c>
       <c r="B37" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="13">
+      <c r="C37" s="9"/>
+      <c r="D37" s="32">
         <v>9</v>
       </c>
-      <c r="E37" s="30" t="s">
+      <c r="E37" s="18" t="s">
         <v>77</v>
       </c>
       <c r="F37" t="s">
@@ -1718,53 +1751,55 @@
       <c r="G37" t="s">
         <v>81</v>
       </c>
-      <c r="H37" s="25">
+      <c r="H37" s="13">
         <v>3</v>
       </c>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14">
+      <c r="I37" s="21">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="18"/>
+      <c r="J37" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
       <c r="B38" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="30"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="18"/>
       <c r="F38" t="s">
         <v>79</v>
       </c>
-      <c r="H38" s="25"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="18"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
       <c r="B39" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="32"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="20"/>
       <c r="F39" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G39" s="2"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="18"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
       <c r="B40" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="29" t="s">
+      <c r="C40" s="10"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="17" t="s">
         <v>82</v>
       </c>
       <c r="F40" t="s">
@@ -1773,92 +1808,96 @@
       <c r="G40" t="s">
         <v>85</v>
       </c>
-      <c r="H40" s="26">
+      <c r="H40" s="15">
         <v>4</v>
       </c>
-      <c r="I40" s="23"/>
+      <c r="I40" s="23">
+        <v>4</v>
+      </c>
       <c r="J40" s="23">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="18"/>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
       <c r="B41" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="30"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="18"/>
       <c r="F41" t="s">
         <v>39</v>
       </c>
-      <c r="H41" s="25"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-    </row>
-    <row r="42" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="11"/>
       <c r="B42" s="6"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="31"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="19"/>
       <c r="F42" s="6" t="s">
         <v>84</v>
       </c>
       <c r="G42" s="7"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="15"/>
-      <c r="J42" s="15"/>
-    </row>
-    <row r="43" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="17" t="s">
+      <c r="H42" s="16"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>86</v>
       </c>
       <c r="B43" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="17"/>
-      <c r="D43" s="13">
+      <c r="C43" s="9"/>
+      <c r="D43" s="32">
         <v>25</v>
       </c>
-      <c r="E43" s="30" t="s">
+      <c r="E43" s="18" t="s">
         <v>87</v>
       </c>
       <c r="F43" t="s">
         <v>74</v>
       </c>
-      <c r="H43" s="25">
+      <c r="H43" s="13">
         <v>1</v>
       </c>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14">
+      <c r="I43" s="21">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="18"/>
+      <c r="J43" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
       <c r="B44" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="18"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="32"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="20"/>
       <c r="F44" s="2" t="s">
         <v>88</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="18"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
       <c r="B45" t="s">
         <v>94</v>
       </c>
-      <c r="C45" s="18"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="29" t="s">
+      <c r="C45" s="10"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="17" t="s">
         <v>89</v>
       </c>
       <c r="F45" t="s">
@@ -1867,76 +1906,78 @@
       <c r="G45" t="s">
         <v>92</v>
       </c>
-      <c r="H45" s="26">
+      <c r="H45" s="15">
         <v>4</v>
       </c>
-      <c r="I45" s="23"/>
+      <c r="I45" s="23">
+        <v>4</v>
+      </c>
       <c r="J45" s="23">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="30"/>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="18"/>
       <c r="F46" t="s">
         <v>36</v>
       </c>
-      <c r="H46" s="25"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="30"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="18"/>
       <c r="F47" t="s">
         <v>90</v>
       </c>
-      <c r="H47" s="25"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="30"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="18"/>
       <c r="F48" t="s">
         <v>80</v>
       </c>
-      <c r="H48" s="25"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-    </row>
-    <row r="49" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="19"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="11"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="31"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="19"/>
       <c r="F49" s="6" t="s">
         <v>91</v>
       </c>
       <c r="G49" s="7"/>
-      <c r="H49" s="27"/>
-      <c r="I49" s="15"/>
-      <c r="J49" s="15"/>
-    </row>
-    <row r="50" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="17" t="s">
+      <c r="H49" s="16"/>
+      <c r="I49" s="24"/>
+      <c r="J49" s="24"/>
+    </row>
+    <row r="50" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
         <v>95</v>
       </c>
       <c r="B50" t="s">
         <v>39</v>
       </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="13">
+      <c r="C50" s="9"/>
+      <c r="D50" s="32">
         <v>79</v>
       </c>
-      <c r="E50" s="30" t="s">
+      <c r="E50" s="18" t="s">
         <v>96</v>
       </c>
       <c r="F50" t="s">
@@ -1945,91 +1986,95 @@
       <c r="G50" t="s">
         <v>98</v>
       </c>
-      <c r="H50" s="25">
+      <c r="H50" s="13">
         <v>4</v>
       </c>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14">
+      <c r="I50" s="21">
+        <v>4</v>
+      </c>
+      <c r="J50" s="21">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" s="18"/>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
       <c r="B51" t="s">
         <v>94</v>
       </c>
-      <c r="C51" s="18"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="32"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="20"/>
       <c r="F51" s="2" t="s">
         <v>97</v>
       </c>
       <c r="G51" s="2"/>
-      <c r="H51" s="28"/>
-      <c r="I51" s="24"/>
-      <c r="J51" s="24"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" s="18"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
       <c r="B52" t="s">
         <v>76</v>
       </c>
-      <c r="C52" s="18"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="29" t="s">
+      <c r="C52" s="10"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="17" t="s">
         <v>99</v>
       </c>
       <c r="F52" t="s">
         <v>18</v>
       </c>
-      <c r="H52" s="26">
+      <c r="H52" s="15">
         <v>1</v>
       </c>
-      <c r="I52" s="23"/>
+      <c r="I52" s="23">
+        <v>1</v>
+      </c>
       <c r="J52" s="23">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="30"/>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="18"/>
       <c r="F53" t="s">
         <v>58</v>
       </c>
-      <c r="H53" s="25"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-    </row>
-    <row r="54" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="19"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="11"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="31"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="19"/>
       <c r="F54" s="6" t="s">
         <v>100</v>
       </c>
       <c r="G54" s="7"/>
-      <c r="H54" s="27"/>
-      <c r="I54" s="15"/>
-      <c r="J54" s="15"/>
-    </row>
-    <row r="55" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="20" t="s">
+      <c r="H54" s="16"/>
+      <c r="I54" s="24"/>
+      <c r="J54" s="24"/>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="12" t="s">
         <v>101</v>
       </c>
       <c r="B55" t="s">
         <v>74</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="C55" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="D55" s="16">
+      <c r="D55" s="29">
         <v>55</v>
       </c>
-      <c r="E55" s="30" t="s">
+      <c r="E55" s="18" t="s">
         <v>104</v>
       </c>
       <c r="F55" t="s">
@@ -2038,146 +2083,182 @@
       <c r="G55" t="s">
         <v>105</v>
       </c>
-      <c r="H55" s="25">
+      <c r="H55" s="13">
         <v>4</v>
       </c>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14">
+      <c r="I55" s="21">
+        <v>5</v>
+      </c>
+      <c r="J55" s="21">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A56" s="20"/>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="12"/>
       <c r="B56" t="s">
         <v>103</v>
       </c>
-      <c r="C56" s="20"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="30"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="18"/>
       <c r="F56" t="s">
         <v>103</v>
       </c>
-      <c r="H56" s="25"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A57" s="20"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="21"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="12"/>
       <c r="B57" t="s">
         <v>76</v>
       </c>
-      <c r="C57" s="20"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="30"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="18"/>
       <c r="F57" t="s">
         <v>76</v>
       </c>
-      <c r="H57" s="25"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" s="20"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="21"/>
+      <c r="J57" s="21"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="12"/>
       <c r="B58" t="s">
         <v>22</v>
       </c>
-      <c r="C58" s="20"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="32"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="20"/>
       <c r="F58" s="2" t="s">
         <v>106</v>
       </c>
       <c r="G58" s="2"/>
-      <c r="H58" s="28"/>
-      <c r="I58" s="24"/>
-      <c r="J58" s="24"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59" s="20"/>
-      <c r="C59" s="20"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="33" t="s">
+      <c r="H58" s="14"/>
+      <c r="I58" s="22"/>
+      <c r="J58" s="22"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="37" t="s">
         <v>107</v>
       </c>
       <c r="F59" t="s">
         <v>74</v>
       </c>
-      <c r="H59" s="25">
+      <c r="H59" s="13">
         <v>5</v>
       </c>
-      <c r="I59" s="16"/>
-      <c r="J59" s="16">
+      <c r="I59" s="29">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A60" s="20"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="33"/>
+      <c r="J59" s="29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="37"/>
       <c r="F60" t="s">
         <v>103</v>
       </c>
-      <c r="H60" s="25"/>
-      <c r="I60" s="16"/>
-      <c r="J60" s="16"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A61" s="20"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="33"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="29"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="37"/>
       <c r="F61" t="s">
         <v>76</v>
       </c>
-      <c r="H61" s="25"/>
-      <c r="I61" s="16"/>
-      <c r="J61" s="16"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A62" s="20"/>
-      <c r="C62" s="20"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="33"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="29"/>
+      <c r="J61" s="29"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="29"/>
+      <c r="E62" s="37"/>
       <c r="F62" t="s">
         <v>22</v>
       </c>
-      <c r="H62" s="25"/>
-      <c r="I62" s="16"/>
-      <c r="J62" s="16"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="29"/>
+      <c r="J62" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="116">
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="A55:A62"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="C7:C13"/>
-    <mergeCell ref="C14:C19"/>
-    <mergeCell ref="C20:C24"/>
-    <mergeCell ref="C25:C30"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A25:A30"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="E37:E39"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="D37:D42"/>
+    <mergeCell ref="D43:D49"/>
+    <mergeCell ref="D50:D54"/>
+    <mergeCell ref="D55:D62"/>
+    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="C55:C62"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
+    <mergeCell ref="E55:E58"/>
+    <mergeCell ref="E59:E62"/>
+    <mergeCell ref="E45:E49"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="A43:A49"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="D7:D13"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="D20:D24"/>
+    <mergeCell ref="D25:D30"/>
+    <mergeCell ref="D31:D36"/>
+    <mergeCell ref="I52:I54"/>
+    <mergeCell ref="J52:J54"/>
+    <mergeCell ref="I55:I58"/>
+    <mergeCell ref="J55:J58"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="J31:J33"/>
+    <mergeCell ref="J14:J17"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="I22:I24"/>
+    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="I59:I62"/>
+    <mergeCell ref="J59:J62"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="J43:J44"/>
+    <mergeCell ref="I45:I49"/>
+    <mergeCell ref="J45:J49"/>
+    <mergeCell ref="I50:I51"/>
+    <mergeCell ref="J50:J51"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="I40:I42"/>
+    <mergeCell ref="J40:J42"/>
     <mergeCell ref="H59:H62"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="J3:J4"/>
@@ -2202,68 +2283,36 @@
     <mergeCell ref="H37:H39"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I59:I62"/>
-    <mergeCell ref="J59:J62"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="J43:J44"/>
-    <mergeCell ref="I45:I49"/>
-    <mergeCell ref="J45:J49"/>
-    <mergeCell ref="I50:I51"/>
-    <mergeCell ref="J50:J51"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J34:J36"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="I40:I42"/>
-    <mergeCell ref="J40:J42"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="D7:D13"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="D20:D24"/>
-    <mergeCell ref="D25:D30"/>
-    <mergeCell ref="D31:D36"/>
-    <mergeCell ref="I52:I54"/>
-    <mergeCell ref="J52:J54"/>
-    <mergeCell ref="I55:I58"/>
-    <mergeCell ref="J55:J58"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="J25:J27"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="J31:J33"/>
-    <mergeCell ref="J14:J17"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="I22:I24"/>
-    <mergeCell ref="J22:J24"/>
-    <mergeCell ref="E52:E54"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="D37:D42"/>
-    <mergeCell ref="D43:D49"/>
-    <mergeCell ref="D50:D54"/>
-    <mergeCell ref="D55:D62"/>
-    <mergeCell ref="C31:C36"/>
-    <mergeCell ref="C55:C62"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="E59:E62"/>
-    <mergeCell ref="E45:E49"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="A43:A49"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="A55:A62"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="C7:C13"/>
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="C25:C30"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A25:A30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E7" r:id="rId1" xr:uid="{DF6C5B22-B422-410A-B22A-3B4DEF6A512C}"/>

</xml_diff>